<commit_message>
Alteração em TravelEasy e Ciclo de Vida
</commit_message>
<xml_diff>
--- a/Modelagem de Sistema - SENAI/KaioMazza_Entregas dos requisitos - Ciclo de vida.xlsx
+++ b/Modelagem de Sistema - SENAI/KaioMazza_Entregas dos requisitos - Ciclo de vida.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaio_mazza\Documents\GitHub\Estudos_Diversos_Programacao\Modelagem de Sistema - SENAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948F8D17-1600-41FD-ADE9-D0E76C1B3B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFA8FF2-B21F-4ECC-8153-5C81A8196429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Prioridade</t>
   </si>
@@ -176,7 +176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -199,12 +199,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -216,10 +242,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -505,13 +535,13 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="F1:H8"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="37.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" style="2" customWidth="1"/>
@@ -519,25 +549,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="5"/>
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -555,9 +582,6 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -575,9 +599,6 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -595,9 +616,6 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -615,9 +633,6 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -654,8 +669,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>